<commit_message>
split primerily end 04-13-18
</commit_message>
<xml_diff>
--- a/view/object/xlsx/create.xlsx
+++ b/view/object/xlsx/create.xlsx
@@ -16,84 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
-    <t xml:space="preserve">canopy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">captor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">caravan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">caress </t>
-  </si>
-  <si>
-    <t xml:space="preserve">caret </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cassock </t>
-  </si>
-  <si>
-    <t xml:space="preserve">catapult </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cater </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cavern </t>
-  </si>
-  <si>
-    <t xml:space="preserve">cease </t>
-  </si>
-  <si>
-    <t xml:space="preserve">chapel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">charitable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">charity </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ক্যানাপি</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেপ্‌টা</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেরাভেন্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কারেস্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেরাট্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেসাক্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেটাপুল্‌ট্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেইটা</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> কেভান্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> সীস্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> চ্যাপল্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> চেরিটেবল্‌</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> চেরিটি</t>
+    <t>ABM</t>
   </si>
 </sst>
 </file>
@@ -432,7 +357,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,63 +371,23 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +411,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,69 +420,19 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A1"/>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A2"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
+      <c r="A3"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
+      <c r="A5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>